<commit_message>
appendix tables and script updated with new 201006 run
</commit_message>
<xml_diff>
--- a/appendix/mean_4ds_accuracy_balanced.xlsx
+++ b/appendix/mean_4ds_accuracy_balanced.xlsx
@@ -569,22 +569,22 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.244</v>
+        <v>0.256</v>
       </c>
       <c r="D5" t="n">
-        <v>0.371</v>
+        <v>0.392</v>
       </c>
       <c r="E5" t="n">
-        <v>0.424</v>
+        <v>0.439</v>
       </c>
       <c r="F5" t="n">
-        <v>0.461</v>
+        <v>0.477</v>
       </c>
       <c r="G5" t="n">
-        <v>0.49</v>
+        <v>0.514</v>
       </c>
       <c r="H5" t="n">
-        <v>0.506</v>
+        <v>0.529</v>
       </c>
     </row>
     <row r="6">
@@ -618,20 +618,20 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>classical-best-embeddings</t>
+          <t>classical-best-embed</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.244</v>
+        <v>0.256</v>
       </c>
       <c r="D7" t="n">
-        <v>0.378</v>
+        <v>0.392</v>
       </c>
       <c r="E7" t="n">
-        <v>0.426</v>
+        <v>0.439</v>
       </c>
       <c r="F7" t="n">
         <v>0.491</v>
@@ -653,22 +653,22 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.237</v>
+        <v>0.246</v>
       </c>
       <c r="D8" t="n">
-        <v>0.464</v>
+        <v>0.48</v>
       </c>
       <c r="E8" t="n">
-        <v>0.533</v>
+        <v>0.522</v>
       </c>
       <c r="F8" t="n">
-        <v>0.592</v>
+        <v>0.583</v>
       </c>
       <c r="G8" t="n">
-        <v>0.626</v>
+        <v>0.625</v>
       </c>
       <c r="H8" t="n">
-        <v>0.636</v>
+        <v>0.633</v>
       </c>
     </row>
     <row r="9">
@@ -678,25 +678,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.352</v>
+        <v>0.359</v>
       </c>
       <c r="C9" t="n">
-        <v>0.436</v>
+        <v>0.47</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5649999999999999</v>
+        <v>0.554</v>
       </c>
       <c r="E9" t="n">
-        <v>0.593</v>
+        <v>0.584</v>
       </c>
       <c r="F9" t="n">
         <v>0.62</v>
       </c>
       <c r="G9" t="n">
-        <v>0.647</v>
+        <v>0.642</v>
       </c>
       <c r="H9" t="n">
-        <v>0.661</v>
+        <v>0.653</v>
       </c>
     </row>
   </sheetData>

</xml_diff>